<commit_message>
Rename and add literature
</commit_message>
<xml_diff>
--- a/practice_xcs.xlsx
+++ b/practice_xcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr backupFile="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="0" windowWidth="25380" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="-75" yWindow="0" windowWidth="25380" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="single" sheetId="27" r:id="rId1"/>
@@ -1096,11 +1096,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="139758976"/>
-        <c:axId val="139785728"/>
+        <c:axId val="85842176"/>
+        <c:axId val="85721856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139758976"/>
+        <c:axId val="85842176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,12 +1125,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139785728"/>
+        <c:crossAx val="85721856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139785728"/>
+        <c:axId val="85721856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1156,7 +1156,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139758976"/>
+        <c:crossAx val="85842176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1170,7 +1170,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000244" l="0.7000000000000014" r="0.7000000000000014" t="0.75000000000000244" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1192,6 +1192,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1219,22 +1220,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>-32.583333333333336</c:v>
+                  <c:v>-32.58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-17.416666666666668</c:v>
+                  <c:v>-17.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-32.583333333333336</c:v>
+                  <c:v>-32.58</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.416666666666668</c:v>
+                  <c:v>17.41</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>32.58</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.416666666666668</c:v>
+                  <c:v>17.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1411,12 +1412,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="89456000"/>
-        <c:axId val="89601536"/>
+        <c:axId val="110569728"/>
+        <c:axId val="110580096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89456000"/>
+        <c:axId val="110569728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,15 +1437,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89601536"/>
+        <c:crossAx val="110580096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89601536"/>
+        <c:axId val="110580096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,23 +1468,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89456000"/>
+        <c:crossAx val="110569728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1505,6 +1508,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1677,10 +1681,10 @@
                   <c:v>46.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.24666666666667</c:v>
+                  <c:v>93.24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88.586666666666673</c:v>
+                  <c:v>88.58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1727,7 +1731,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>97.909000000000006</c:v>
+                  <c:v>97.902000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1775,7 +1779,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>97.909000000000006</c:v>
+                  <c:v>97.902000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1784,12 +1788,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="89765760"/>
-        <c:axId val="89653248"/>
+        <c:axId val="110752512"/>
+        <c:axId val="110754432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89765760"/>
+        <c:axId val="110752512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1810,15 +1813,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89653248"/>
+        <c:crossAx val="110754432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89653248"/>
+        <c:axId val="110754432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1840,23 +1844,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89765760"/>
+        <c:crossAx val="110752512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1878,6 +1884,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1941,19 +1948,19 @@
                   <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>217.58333333333331</c:v>
+                  <c:v>217.58</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>214.33333333333331</c:v>
+                  <c:v>214.33</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>217.25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>232.41666666666669</c:v>
+                  <c:v>232.41</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>235.66666666666669</c:v>
+                  <c:v>235.66</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>232.75</c:v>
@@ -2065,10 +2072,10 @@
                   <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>219.66666666666669</c:v>
+                  <c:v>219.66</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>230.33333333333331</c:v>
+                  <c:v>230.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2092,10 +2099,10 @@
                   <c:v>46.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.24666666666667</c:v>
+                  <c:v>93.24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88.586666666666673</c:v>
+                  <c:v>88.58</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>58.42</c:v>
@@ -2148,7 +2155,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>97.909000000000006</c:v>
+                  <c:v>97.902000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2196,7 +2203,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>97.909000000000006</c:v>
+                  <c:v>97.902000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2205,12 +2212,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="89710976"/>
-        <c:axId val="89712896"/>
+        <c:axId val="110685184"/>
+        <c:axId val="111289472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89710976"/>
+        <c:axId val="110685184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2231,15 +2237,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89712896"/>
+        <c:crossAx val="111289472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89712896"/>
+        <c:axId val="111289472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2261,23 +2268,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89710976"/>
+        <c:crossAx val="110685184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2299,6 +2308,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2494,12 +2504,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="112245376"/>
-        <c:axId val="112255744"/>
+        <c:axId val="117474816"/>
+        <c:axId val="117476736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112245376"/>
+        <c:axId val="117474816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2520,15 +2529,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112255744"/>
+        <c:crossAx val="117476736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112255744"/>
+        <c:axId val="117476736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2550,23 +2560,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112245376"/>
+        <c:crossAx val="117474816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2588,6 +2600,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2783,12 +2796,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="118400128"/>
-        <c:axId val="118402048"/>
+        <c:axId val="117555200"/>
+        <c:axId val="117557120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118400128"/>
+        <c:axId val="117555200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2809,15 +2821,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118402048"/>
+        <c:crossAx val="117557120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118402048"/>
+        <c:axId val="117557120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2839,23 +2852,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118400128"/>
+        <c:crossAx val="117555200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3073,12 +3088,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="112270720"/>
-        <c:axId val="112276992"/>
+        <c:axId val="102193408"/>
+        <c:axId val="102207872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112270720"/>
+        <c:axId val="102193408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3103,12 +3117,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112276992"/>
+        <c:crossAx val="102207872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112276992"/>
+        <c:axId val="102207872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3134,7 +3148,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112270720"/>
+        <c:crossAx val="102193408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3148,7 +3162,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3354,11 +3368,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="72110464"/>
-        <c:axId val="72112384"/>
+        <c:axId val="85765504"/>
+        <c:axId val="85771776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72110464"/>
+        <c:axId val="85765504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3383,12 +3397,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72112384"/>
+        <c:crossAx val="85771776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72112384"/>
+        <c:axId val="85771776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3414,7 +3428,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72110464"/>
+        <c:crossAx val="85765504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3428,7 +3442,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3694,12 +3708,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="85617664"/>
-        <c:axId val="85628032"/>
+        <c:axId val="101148544"/>
+        <c:axId val="101158912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85617664"/>
+        <c:axId val="101148544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3724,12 +3737,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85628032"/>
+        <c:crossAx val="101158912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85628032"/>
+        <c:axId val="101158912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3755,7 +3768,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85617664"/>
+        <c:crossAx val="101148544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3769,7 +3782,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3791,6 +3804,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4034,12 +4048,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="85685760"/>
-        <c:axId val="85687680"/>
+        <c:axId val="101232640"/>
+        <c:axId val="101234560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85685760"/>
+        <c:axId val="101232640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4060,15 +4073,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85687680"/>
+        <c:crossAx val="101234560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85687680"/>
+        <c:axId val="101234560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4090,23 +4104,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85685760"/>
+        <c:crossAx val="101232640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4128,6 +4144,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4371,12 +4388,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="86585344"/>
-        <c:axId val="86587264"/>
+        <c:axId val="101259520"/>
+        <c:axId val="101294464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86585344"/>
+        <c:axId val="101259520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4397,15 +4413,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86587264"/>
+        <c:crossAx val="101294464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86587264"/>
+        <c:axId val="101294464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4427,23 +4444,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86585344"/>
+        <c:crossAx val="101259520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4465,6 +4484,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4702,12 +4722,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="87328640"/>
-        <c:axId val="87334912"/>
+        <c:axId val="101798656"/>
+        <c:axId val="101800576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87328640"/>
+        <c:axId val="101798656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4728,15 +4747,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87334912"/>
+        <c:crossAx val="101800576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87334912"/>
+        <c:axId val="101800576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4758,23 +4778,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87328640"/>
+        <c:crossAx val="101798656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4796,6 +4818,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5033,12 +5056,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="87372160"/>
-        <c:axId val="87374080"/>
+        <c:axId val="101903360"/>
+        <c:axId val="101721216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87372160"/>
+        <c:axId val="101903360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5059,15 +5081,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87374080"/>
+        <c:crossAx val="101721216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87374080"/>
+        <c:axId val="101721216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5089,23 +5112,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87372160"/>
+        <c:crossAx val="101903360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5127,6 +5152,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5364,12 +5390,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="87419520"/>
-        <c:axId val="87520000"/>
+        <c:axId val="108430848"/>
+        <c:axId val="108432768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87419520"/>
+        <c:axId val="108430848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5390,15 +5415,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87520000"/>
+        <c:crossAx val="108432768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87520000"/>
+        <c:axId val="108432768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5420,23 +5446,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87419520"/>
+        <c:crossAx val="108430848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5458,6 +5486,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5683,12 +5712,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="89515136"/>
-        <c:axId val="89517056"/>
+        <c:axId val="108335104"/>
+        <c:axId val="108337024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89515136"/>
+        <c:axId val="108335104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5709,15 +5737,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89517056"/>
+        <c:crossAx val="108337024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89517056"/>
+        <c:axId val="108337024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5739,23 +5768,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89515136"/>
+        <c:crossAx val="108335104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000107" r="0.70000000000000107" t="0.75000000000000211" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6583,8 +6614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -7002,7 +7033,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6:Q6"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -7147,7 +7178,7 @@
         <v>38</v>
       </c>
       <c r="D5" s="52">
-        <v>-32.583333333333336</v>
+        <v>-32.58</v>
       </c>
       <c r="E5" s="52">
         <v>28.5</v>
@@ -7156,10 +7187,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="52">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="H5" s="52">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="I5" s="52">
         <v>115</v>
@@ -7202,7 +7233,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="52">
-        <v>-17.416666666666668</v>
+        <v>-17.41</v>
       </c>
       <c r="E6" s="52">
         <v>34.5</v>
@@ -7211,10 +7242,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="52">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="H6" s="52">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="I6" s="52">
         <v>115</v>
@@ -7256,7 +7287,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="51">
-        <v>-32.583333333333336</v>
+        <v>-32.58</v>
       </c>
       <c r="E7" s="51">
         <v>40.5</v>
@@ -7265,10 +7296,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="51">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="H7" s="51">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="I7" s="51">
         <v>115</v>
@@ -7298,7 +7329,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="52">
-        <v>17.416666666666668</v>
+        <v>17.41</v>
       </c>
       <c r="E8" s="52">
         <v>28.5</v>
@@ -7307,10 +7338,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="52">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="H8" s="52">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="I8" s="52">
         <v>115</v>
@@ -7350,10 +7381,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="52">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="H9" s="52">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="I9" s="52">
         <v>115</v>
@@ -7379,7 +7410,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="51">
-        <v>17.416666666666668</v>
+        <v>17.41</v>
       </c>
       <c r="E10" s="51">
         <v>40.5</v>
@@ -7388,10 +7419,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="51">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="H10" s="51">
-        <v>1.2929999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="I10" s="51">
         <v>115</v>
@@ -7571,7 +7602,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6:Q6"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -7753,7 +7784,7 @@
       </c>
       <c r="P5" s="32">
         <f>MAX(E5:E25,N5:N26)*1.05</f>
-        <v>97.909000000000006</v>
+        <v>97.902000000000001</v>
       </c>
       <c r="Q5" s="32">
         <f>B13</f>
@@ -7959,7 +7990,7 @@
         <v>136</v>
       </c>
       <c r="N9" s="74">
-        <v>93.24666666666667</v>
+        <v>93.24</v>
       </c>
       <c r="O9" s="79">
         <v>1</v>
@@ -8006,7 +8037,7 @@
         <v>164</v>
       </c>
       <c r="N10" s="74">
-        <v>88.586666666666673</v>
+        <v>88.58</v>
       </c>
       <c r="O10" s="79">
         <v>1</v>
@@ -8032,10 +8063,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="74">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H11" s="74">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I11" s="74">
         <v>345</v>
@@ -8068,10 +8099,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="74">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H12" s="74">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I12" s="74">
         <v>345</v>
@@ -8104,10 +8135,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="73">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H13" s="73">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I13" s="73">
         <v>345</v>
@@ -8140,10 +8171,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="74">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H14" s="74">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I14" s="74">
         <v>115</v>
@@ -8174,10 +8205,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="74">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H15" s="74">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I15" s="74">
         <v>115</v>
@@ -8206,10 +8237,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="73">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H16" s="73">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I16" s="73">
         <v>115</v>
@@ -8312,7 +8343,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -8494,7 +8525,7 @@
       </c>
       <c r="P5" s="32">
         <f>MAX(E5:E25,N5:N26)*1.05</f>
-        <v>97.909000000000006</v>
+        <v>97.902000000000001</v>
       </c>
       <c r="Q5" s="32">
         <f>B13</f>
@@ -8700,7 +8731,7 @@
         <v>136</v>
       </c>
       <c r="N9" s="74">
-        <v>93.24666666666667</v>
+        <v>93.24</v>
       </c>
       <c r="O9" s="79">
         <v>1</v>
@@ -8747,7 +8778,7 @@
         <v>164</v>
       </c>
       <c r="N10" s="74">
-        <v>88.586666666666673</v>
+        <v>88.58</v>
       </c>
       <c r="O10" s="79">
         <v>1</v>
@@ -8773,10 +8804,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="60">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H11" s="60">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I11" s="60">
         <v>345</v>
@@ -8791,7 +8822,7 @@
         <v>36</v>
       </c>
       <c r="M11" s="74">
-        <v>219.66666666666669</v>
+        <v>219.66</v>
       </c>
       <c r="N11" s="74">
         <v>58.42</v>
@@ -8820,10 +8851,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="60">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H12" s="60">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I12" s="60">
         <v>345</v>
@@ -8838,7 +8869,7 @@
         <v>69</v>
       </c>
       <c r="M12" s="74">
-        <v>230.33333333333331</v>
+        <v>230.33</v>
       </c>
       <c r="N12" s="74">
         <v>58.42</v>
@@ -8867,10 +8898,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="59">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H13" s="59">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I13" s="59">
         <v>345</v>
@@ -8904,10 +8935,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="60">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H14" s="60">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I14" s="60">
         <v>115</v>
@@ -8939,10 +8970,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="60">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H15" s="60">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I15" s="60">
         <v>115</v>
@@ -8972,10 +9003,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="59">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="H16" s="59">
-        <v>1.7350000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="I16" s="59">
         <v>115</v>
@@ -8994,7 +9025,7 @@
         <v>38</v>
       </c>
       <c r="D17" s="60">
-        <v>217.58333333333331</v>
+        <v>217.58</v>
       </c>
       <c r="E17" s="60">
         <v>20.170000000000002</v>
@@ -9024,7 +9055,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="60">
-        <v>214.33333333333331</v>
+        <v>214.33</v>
       </c>
       <c r="E18" s="60">
         <v>32.17</v>
@@ -9084,7 +9115,7 @@
         <v>62</v>
       </c>
       <c r="D20" s="60">
-        <v>232.41666666666669</v>
+        <v>232.41</v>
       </c>
       <c r="E20" s="60">
         <v>20.170000000000002</v>
@@ -9115,7 +9146,7 @@
         <v>63</v>
       </c>
       <c r="D21" s="60">
-        <v>235.66666666666669</v>
+        <v>235.66</v>
       </c>
       <c r="E21" s="60">
         <v>32.17</v>
@@ -10189,7 +10220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -10668,7 +10699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -11097,7 +11128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -13032,7 +13063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P6" sqref="P6:Q6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Build target_fields() function with bisection
</commit_message>
<xml_diff>
--- a/practice_xcs.xlsx
+++ b/practice_xcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr backupFile="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="0" windowWidth="25380" windowHeight="16440" activeTab="7"/>
+    <workbookView xWindow="-75" yWindow="0" windowWidth="25380" windowHeight="16440" firstSheet="3" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="single" sheetId="27" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="raise2" sheetId="24" r:id="rId18"/>
     <sheet name="raise3" sheetId="25" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -934,7 +934,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1112,11 +1111,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="139653120"/>
-        <c:axId val="139655424"/>
+        <c:axId val="71993600"/>
+        <c:axId val="75301248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139653120"/>
+        <c:axId val="71993600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1137,16 +1136,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139655424"/>
+        <c:crossAx val="75301248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139655424"/>
+        <c:axId val="75301248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,25 +1166,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139653120"/>
+        <c:crossAx val="71993600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1446,11 +1442,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55584640"/>
-        <c:axId val="55590912"/>
+        <c:axId val="73029888"/>
+        <c:axId val="73048448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55584640"/>
+        <c:axId val="73029888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,12 +1471,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55590912"/>
+        <c:crossAx val="73048448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55590912"/>
+        <c:axId val="73048448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1506,7 +1502,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55584640"/>
+        <c:crossAx val="73029888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1520,7 +1516,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1780,11 +1776,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55605888"/>
-        <c:axId val="55616256"/>
+        <c:axId val="73337856"/>
+        <c:axId val="73352320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55605888"/>
+        <c:axId val="73337856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1809,12 +1805,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55616256"/>
+        <c:crossAx val="73352320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55616256"/>
+        <c:axId val="73352320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1840,7 +1836,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55605888"/>
+        <c:crossAx val="73337856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1854,7 +1850,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1876,7 +1872,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2114,11 +2109,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55754112"/>
-        <c:axId val="55760384"/>
+        <c:axId val="73441280"/>
+        <c:axId val="73443200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55754112"/>
+        <c:axId val="73441280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2139,16 +2134,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55760384"/>
+        <c:crossAx val="73443200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55760384"/>
+        <c:axId val="73443200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2170,25 +2164,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55754112"/>
+        <c:crossAx val="73441280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2210,7 +2202,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2436,11 +2427,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55869824"/>
-        <c:axId val="55871744"/>
+        <c:axId val="73491200"/>
+        <c:axId val="73493120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55869824"/>
+        <c:axId val="73491200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2461,16 +2452,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55871744"/>
+        <c:crossAx val="73493120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55871744"/>
+        <c:axId val="73493120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2492,25 +2482,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55869824"/>
+        <c:crossAx val="73491200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2532,7 +2520,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2752,11 +2739,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="69096576"/>
-        <c:axId val="69098496"/>
+        <c:axId val="74151424"/>
+        <c:axId val="74153344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69096576"/>
+        <c:axId val="74151424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2777,16 +2764,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69098496"/>
+        <c:crossAx val="74153344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69098496"/>
+        <c:axId val="74153344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,25 +2794,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69096576"/>
+        <c:crossAx val="74151424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3128,11 +3112,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="70915968"/>
-        <c:axId val="70930432"/>
+        <c:axId val="74369280"/>
+        <c:axId val="74375552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70915968"/>
+        <c:axId val="74369280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3157,12 +3141,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70930432"/>
+        <c:crossAx val="74375552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70930432"/>
+        <c:axId val="74375552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3188,7 +3172,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70915968"/>
+        <c:crossAx val="74369280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3202,7 +3186,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3552,11 +3536,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="71387776"/>
-        <c:axId val="71574272"/>
+        <c:axId val="74866048"/>
+        <c:axId val="74876416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71387776"/>
+        <c:axId val="74866048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3581,12 +3565,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71574272"/>
+        <c:crossAx val="74876416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71574272"/>
+        <c:axId val="74876416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3612,7 +3596,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71387776"/>
+        <c:crossAx val="74866048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3626,7 +3610,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3844,11 +3828,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="71605632"/>
-        <c:axId val="71616000"/>
+        <c:axId val="74920320"/>
+        <c:axId val="74922240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71605632"/>
+        <c:axId val="74920320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3873,12 +3857,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71616000"/>
+        <c:crossAx val="74922240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71616000"/>
+        <c:axId val="74922240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3904,7 +3888,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71605632"/>
+        <c:crossAx val="74920320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3918,7 +3902,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4136,11 +4120,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="71807360"/>
-        <c:axId val="71809280"/>
+        <c:axId val="75015296"/>
+        <c:axId val="75017216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71807360"/>
+        <c:axId val="75015296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4165,12 +4149,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71809280"/>
+        <c:crossAx val="75017216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71809280"/>
+        <c:axId val="75017216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4196,7 +4180,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71807360"/>
+        <c:crossAx val="75015296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4210,7 +4194,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4428,11 +4412,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="71857280"/>
-        <c:axId val="71859200"/>
+        <c:axId val="75224960"/>
+        <c:axId val="75325440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71857280"/>
+        <c:axId val="75224960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4457,12 +4441,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71859200"/>
+        <c:crossAx val="75325440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71859200"/>
+        <c:axId val="75325440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4488,7 +4472,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71857280"/>
+        <c:crossAx val="75224960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4502,7 +4486,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4708,11 +4692,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55097984"/>
-        <c:axId val="55100160"/>
+        <c:axId val="76708096"/>
+        <c:axId val="76796672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55097984"/>
+        <c:axId val="76708096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4737,12 +4721,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55100160"/>
+        <c:crossAx val="76796672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55100160"/>
+        <c:axId val="76796672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4768,7 +4752,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55097984"/>
+        <c:crossAx val="76708096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4782,7 +4766,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000162" r="0.70000000000000162" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5048,11 +5032,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55115136"/>
-        <c:axId val="55252480"/>
+        <c:axId val="116417664"/>
+        <c:axId val="126937344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55115136"/>
+        <c:axId val="116417664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5077,12 +5061,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55252480"/>
+        <c:crossAx val="126937344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55252480"/>
+        <c:axId val="126937344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5108,7 +5092,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55115136"/>
+        <c:crossAx val="116417664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5122,7 +5106,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5388,11 +5372,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55509376"/>
-        <c:axId val="55511296"/>
+        <c:axId val="70365952"/>
+        <c:axId val="70367872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55509376"/>
+        <c:axId val="70365952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5417,12 +5401,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55511296"/>
+        <c:crossAx val="70367872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55511296"/>
+        <c:axId val="70367872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5448,7 +5432,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55509376"/>
+        <c:crossAx val="70365952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5462,7 +5446,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5728,11 +5712,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="71590656"/>
-        <c:axId val="71592576"/>
+        <c:axId val="71977216"/>
+        <c:axId val="71999872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71590656"/>
+        <c:axId val="71977216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5757,12 +5741,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71592576"/>
+        <c:crossAx val="71999872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71592576"/>
+        <c:axId val="71999872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5788,7 +5772,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71590656"/>
+        <c:crossAx val="71977216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5802,7 +5786,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000162" r="0.70000000000000162" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6068,11 +6052,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="75201920"/>
-        <c:axId val="75216384"/>
+        <c:axId val="72252416"/>
+        <c:axId val="72258688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75201920"/>
+        <c:axId val="72252416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6097,12 +6081,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75216384"/>
+        <c:crossAx val="72258688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75216384"/>
+        <c:axId val="72258688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6128,7 +6112,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75201920"/>
+        <c:crossAx val="72252416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6142,7 +6126,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6408,11 +6392,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="82998400"/>
-        <c:axId val="83000320"/>
+        <c:axId val="72843264"/>
+        <c:axId val="72845184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82998400"/>
+        <c:axId val="72843264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6437,12 +6421,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83000320"/>
+        <c:crossAx val="72845184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83000320"/>
+        <c:axId val="72845184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6468,7 +6452,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82998400"/>
+        <c:crossAx val="72843264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6482,7 +6466,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000162" r="0.70000000000000162" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6504,7 +6488,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -6748,11 +6731,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="83377536"/>
-        <c:axId val="83392000"/>
+        <c:axId val="72909568"/>
+        <c:axId val="72911488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83377536"/>
+        <c:axId val="72909568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6773,16 +6756,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83392000"/>
+        <c:crossAx val="72911488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83392000"/>
+        <c:axId val="72911488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6804,25 +6786,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83377536"/>
+        <c:crossAx val="72909568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000162" r="0.70000000000000162" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6844,7 +6824,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -7088,11 +7067,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55530624"/>
-        <c:axId val="55532544"/>
+        <c:axId val="72963584"/>
+        <c:axId val="72965504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55530624"/>
+        <c:axId val="72963584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7113,16 +7092,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55532544"/>
+        <c:crossAx val="72965504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55532544"/>
+        <c:axId val="72965504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7144,25 +7122,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55530624"/>
+        <c:crossAx val="72963584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000129" r="0.70000000000000129" t="0.75000000000000233" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11631,7 +11607,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -12371,8 +12347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -15158,7 +15134,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -15802,7 +15778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
@@ -16448,7 +16424,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K13"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -18367,7 +18343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>

</xml_diff>